<commit_message>
erste Tests mit Spitälern
</commit_message>
<xml_diff>
--- a/Gemeinden_Graubünden.xlsx
+++ b/Gemeinden_Graubünden.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marina Frei\Documents\Studium\Bachelorarbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA0FAFB-C13B-4B77-A98C-64A3C4FF7D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802DB43D-8D3E-4F78-8BFD-3EB6431662A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -763,8 +763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -842,10 +842,10 @@
         <v>14</v>
       </c>
       <c r="L2">
-        <v>46.248198761722151</v>
+        <v>46.2481987617222</v>
       </c>
       <c r="M2">
-        <v>9.1490454400061836</v>
+        <v>9.14904544000618</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
@@ -1990,7 +1990,7 @@
         <v>41</v>
       </c>
       <c r="L30">
-        <v>46.828750350264713</v>
+        <v>46.828750350264698</v>
       </c>
       <c r="M30">
         <v>9.3628265761013054</v>
@@ -2031,10 +2031,10 @@
         <v>49</v>
       </c>
       <c r="L31" s="2">
-        <v>46.960616655461827</v>
+        <v>46.960616655461799</v>
       </c>
       <c r="M31" s="2">
-        <v>10.395484762810829</v>
+        <v>10.395484762810799</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.35">
@@ -2195,10 +2195,10 @@
         <v>51</v>
       </c>
       <c r="L35">
-        <v>46.491642104950323</v>
+        <v>46.491642104950301</v>
       </c>
       <c r="M35">
-        <v>9.9046184639690633</v>
+        <v>9.9046184639690598</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
verschiedene Tests mit zwei Gemeinden und Distanz/Fahrzeit
</commit_message>
<xml_diff>
--- a/Gemeinden_Graubünden.xlsx
+++ b/Gemeinden_Graubünden.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marina Frei\Documents\Studium\Bachelorarbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802DB43D-8D3E-4F78-8BFD-3EB6431662A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A098799-B76B-480B-B85E-45E5671074A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -764,7 +777,7 @@
   <dimension ref="A1:M101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>